<commit_message>
Handled an exception and Corrected the spacing in the columns
</commit_message>
<xml_diff>
--- a/BalanceSheet/BalanceSheetViewModel/Docs/AccountDefinitionFormat.xlsx
+++ b/BalanceSheet/BalanceSheetViewModel/Docs/AccountDefinitionFormat.xlsx
@@ -17,65 +17,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="26">
   <si>
     <t>Account</t>
   </si>
   <si>
-    <t>BaSBIAcc12345678</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
     <t>Capital</t>
   </si>
   <si>
-    <t>Xsalary</t>
-  </si>
-  <si>
-    <t>XSalaryDedn</t>
-  </si>
-  <si>
     <t>Salary</t>
   </si>
   <si>
-    <t>BaCitiAcc98765432</t>
-  </si>
-  <si>
-    <t>XSalary</t>
-  </si>
-  <si>
-    <t>InvNPS</t>
-  </si>
-  <si>
-    <t>InvPPFSBI</t>
-  </si>
-  <si>
-    <t>XRentHouseSmrithiWA307</t>
-  </si>
-  <si>
-    <t>EquitySharesLarsenAndToubro</t>
-  </si>
-  <si>
-    <t>IncEquitySharesLarsenAndToubro</t>
-  </si>
-  <si>
-    <t>IncIntPPF</t>
-  </si>
-  <si>
-    <t>IOUiPersonX</t>
-  </si>
-  <si>
-    <t>EquitySharesMandM</t>
-  </si>
-  <si>
     <t>InvCoMfICICIPruDynamic</t>
   </si>
   <si>
-    <t>IOUiPersonY</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -98,21 +56,70 @@
   </si>
   <si>
     <t>Liability</t>
+  </si>
+  <si>
+    <t>Bank Citi Acc#98765432</t>
+  </si>
+  <si>
+    <t>Bank SBI Acc#12345678</t>
+  </si>
+  <si>
+    <t>Inc Equity Shares Larsen&amp;Toubro</t>
+  </si>
+  <si>
+    <t>Inc Int PPF</t>
+  </si>
+  <si>
+    <t>X Rent House Smrithi WA307</t>
+  </si>
+  <si>
+    <t>X Salary</t>
+  </si>
+  <si>
+    <t>X Salary Dedn</t>
+  </si>
+  <si>
+    <t>Equity Shares Larsen&amp;Toubro</t>
+  </si>
+  <si>
+    <t>Inv NPS</t>
+  </si>
+  <si>
+    <t>Inv PPF SBI</t>
+  </si>
+  <si>
+    <t>IOUi PersonX</t>
+  </si>
+  <si>
+    <t>IOUi PersonY</t>
+  </si>
+  <si>
+    <t>Equity Shares M&amp;M</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -138,15 +145,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -438,9 +450,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -449,223 +463,212 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="C11" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C12" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+    <row r="16" spans="1:3">
+      <c r="A16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="C16" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="C17" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="C18" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C18" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" t="s">
-        <v>2</v>
+      <c r="C19" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>